<commit_message>
Adding structural analysis example work
</commit_message>
<xml_diff>
--- a/examples/models/BigBurger.xlsx
+++ b/examples/models/BigBurger.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
   <si>
     <t xml:space="preserve">*Alts</t>
   </si>
@@ -47,196 +47,175 @@
     <t xml:space="preserve">Time Horiz</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1 McDon~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1 White~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1 Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1 Nutri~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1 Perso~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1 Speed~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1 Subs</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1 Short~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2 Burge~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2 Blue ~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2 Produ~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2 Recyc~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2 Food ~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2 Seati~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2 Chick~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2 Mediu~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3 Wendy~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3 Stude~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3 Locat~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3 Waste~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3 Site ~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3 Parki~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3 Pizza</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4 Famil~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4 Deals</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4 Over ~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4 Deliv~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4 Mexic~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5 Drive~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5 Chine~</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6 Steak</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7 Diners</t>
-  </si>
-  <si>
     <t xml:space="preserve">1 McDon~</t>
   </si>
   <si>
+    <t xml:space="preserve">1 White~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Nutri~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Perso~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Speed~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Subs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Short~</t>
+  </si>
+  <si>
     <t xml:space="preserve">2 Burge~</t>
   </si>
   <si>
+    <t xml:space="preserve">2 Blue ~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Produ~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Recyc~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Food ~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Seati~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Chick~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Mediu~</t>
+  </si>
+  <si>
     <t xml:space="preserve">3 Wendy~</t>
   </si>
   <si>
-    <t xml:space="preserve">1 White~</t>
+    <t xml:space="preserve">3 Stude~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Locat~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Waste~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Site ~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Parki~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Pizza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Famil~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Deals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Over ~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Deliv~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Mexic~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Drive~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Chine~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 Steak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 Diners</t>
   </si>
   <si>
     <t xml:space="preserve">2 Blue ~ 3</t>
   </si>
   <si>
-    <t xml:space="preserve"> Stude~</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 Famil~</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Produ~</t>
+    <t xml:space="preserve">Stude~</t>
   </si>
   <si>
     <t xml:space="preserve">3 Locat~ 4</t>
   </si>
   <si>
-    <t xml:space="preserve"> Deals  1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nutri~ 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Recyc~ 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Waste~ 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Over ~ 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Perso~ 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Food ~ 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Site ~ 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Speed~ 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Seati~ 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Parki~ 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Deliv~ 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Drive~ 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Subs   2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Chick~ 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pizza  4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mexic~ 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Chine~ 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Steak  7</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Diners 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Short~ 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mediu~</t>
+    <t xml:space="preserve">Deals  1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nutri~ 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recyc~ 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waste~ 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Over ~ 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perso~ 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food ~ 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Site ~ 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speed~ 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seati~ 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parki~ 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deliv~ 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drive~ 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subs   2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chick~ 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pizza  4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mexic~ 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chine~ 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steak  7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diners 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Short~ 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mediu~</t>
   </si>
 </sst>
 </file>
@@ -251,6 +230,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -335,7 +315,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A33 G1 L1:AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -503,7 +483,7 @@
   <dimension ref="A1:AG33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A33 G1 L1:AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -513,100 +493,100 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="H1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="N1" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="O1" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="P1" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="Q1" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="R1" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="S1" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="T1" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="U1" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="V1" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="W1" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="X1" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="Y1" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="Z1" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="AA1" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="AB1" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="AC1" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="AD1" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="AE1" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="AF1" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="AG1" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="AA1" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB1" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC1" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD1" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="AE1" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF1" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="AG1" s="0" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3844,7 +3824,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>